<commit_message>
ticket 171: ajustado el nombre del archivo de incremento de claro, segun comentario 579
</commit_message>
<xml_diff>
--- a/public/uploads/${ID_ORDEN_SERVICIO} Orden Upgrade ${ID_ORDEN_SERVICIO_LETRAS} ${NODO_CIU_NOMBRE} ${ID_SERVICIO}.xlsx
+++ b/public/uploads/${ID_ORDEN_SERVICIO} Orden Upgrade ${ID_ORDEN_SERVICIO_LETRAS} ${NODO_CIU_NOMBRE} ${ID_SERVICIO}.xlsx
@@ -56,6 +56,7 @@
         <sz val="3.9"/>
         <rFont val=".AppleSystemUIFont"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">﻿</t>
     </r>
@@ -66,7 +67,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">${ID_ORDEN_SERVICIO}</t>
+      <t xml:space="preserve">${ID_SERVICIO} </t>
     </r>
   </si>
   <si>
@@ -132,6 +133,7 @@
       <sz val="3.9"/>
       <name val=".AppleSystemUIFont"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -416,7 +418,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -442,7 +444,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>